<commit_message>
code cleaning in StockPicker.py
</commit_message>
<xml_diff>
--- a/datatickers123.xlsx
+++ b/datatickers123.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,17 +546,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NYMX</t>
+          <t>MAA</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2759</v>
+        <v>24</v>
       </c>
       <c r="E2" t="n">
-        <v>-4999.308</v>
+        <v>-4920.96</v>
       </c>
       <c r="F2" t="n">
-        <v>4999.308</v>
+        <v>4920.96</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -565,46 +565,624 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Nymox Pharmaceutical Corporation</t>
+          <t>Mid-America Apartment Communities, Inc.</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>2455.510289430618</v>
+        <v>867.840087890625</v>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
+          <t>2021-10-14</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>1.0925</v>
+      </c>
+      <c r="M2" t="n">
+        <v>203.98</v>
+      </c>
+      <c r="N2" t="n">
+        <v>205.04</v>
+      </c>
+      <c r="O2" t="n">
+        <v>203.04</v>
+      </c>
+      <c r="P2" t="n">
+        <v>205.97</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>119.21</v>
+      </c>
+      <c r="R2" t="n">
+        <v>207.69</v>
+      </c>
+      <c r="S2" t="n">
+        <v>197.28555</v>
+      </c>
+      <c r="T2" t="n">
+        <v>181.94092</v>
+      </c>
+      <c r="U2" t="n">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TGTX</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>157</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-4989.46</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4989.46</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>TG Therapeutics, Inc.</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>1099.000074863434</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>-</t>
         </is>
       </c>
-      <c r="L2" t="n">
+      <c r="L3" t="n">
         <v>0</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M3" t="n">
+        <v>33.43</v>
+      </c>
+      <c r="N3" t="n">
+        <v>31.78</v>
+      </c>
+      <c r="O3" t="n">
+        <v>31.46</v>
+      </c>
+      <c r="P3" t="n">
+        <v>33.44</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>21.058</v>
+      </c>
+      <c r="R3" t="n">
+        <v>56.74</v>
+      </c>
+      <c r="S3" t="n">
+        <v>32.713055</v>
+      </c>
+      <c r="T3" t="n">
+        <v>33.39571</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CIB</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>150</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-4968</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4968</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Bancolombia S.A.</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>2503.500366210938</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2021-09-28</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>0.3498</v>
+      </c>
+      <c r="M4" t="n">
+        <v>33.08</v>
+      </c>
+      <c r="N4" t="n">
+        <v>33.12</v>
+      </c>
+      <c r="O4" t="n">
+        <v>32.48</v>
+      </c>
+      <c r="P4" t="n">
+        <v>33.22</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>27.64</v>
+      </c>
+      <c r="R4" t="n">
+        <v>42</v>
+      </c>
+      <c r="S4" t="n">
+        <v>35.11778</v>
+      </c>
+      <c r="T4" t="n">
+        <v>31.715036</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BOH</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>57</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-4984.650000000001</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4984.650000000001</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Bank of Hawaii Corporation</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>1586.880226135254</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2021-11-29</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>0.4705</v>
+      </c>
+      <c r="M5" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="N5" t="n">
+        <v>87.45</v>
+      </c>
+      <c r="O5" t="n">
+        <v>86.52500000000001</v>
+      </c>
+      <c r="P5" t="n">
+        <v>88.06</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>73.11</v>
+      </c>
+      <c r="R5" t="n">
+        <v>99.09999999999999</v>
+      </c>
+      <c r="S5" t="n">
+        <v>84.674446</v>
+      </c>
+      <c r="T5" t="n">
+        <v>85.42843999999999</v>
+      </c>
+      <c r="U5" t="n">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CLSD</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1022</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-4997.58</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4997.58</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Clearside Biomedical, Inc.</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>1870.260043859482</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="N6" t="n">
+        <v>4.89</v>
+      </c>
+      <c r="O6" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="P6" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="R6" t="n">
+        <v>7.73</v>
+      </c>
+      <c r="S6" t="n">
+        <v>5.463611</v>
+      </c>
+      <c r="T6" t="n">
+        <v>4.901454</v>
+      </c>
+      <c r="U6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>HASI</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>78</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-4998.24</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4998.24</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Hannon Armstrong Sustainable Infrastructure Capital, Inc.</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>1024.140083312988</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2021-12-27</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>1.2523</v>
+      </c>
+      <c r="M7" t="n">
+        <v>63.07</v>
+      </c>
+      <c r="N7" t="n">
+        <v>64.08</v>
+      </c>
+      <c r="O7" t="n">
+        <v>62.94</v>
+      </c>
+      <c r="P7" t="n">
+        <v>64.23999999999999</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>44.69</v>
+      </c>
+      <c r="R7" t="n">
+        <v>72.42</v>
+      </c>
+      <c r="S7" t="n">
+        <v>58.64528</v>
+      </c>
+      <c r="T7" t="n">
+        <v>55.591843</v>
+      </c>
+      <c r="U7" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>AVAL</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>886</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-4997.04</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4997.04</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Grupo Aval Acciones y Valores S.A.</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>2498.52015209198</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2021-11-29</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>0.4273</v>
+      </c>
+      <c r="M8" t="n">
+        <v>5.62</v>
+      </c>
+      <c r="N8" t="n">
+        <v>5.64</v>
+      </c>
+      <c r="O8" t="n">
+        <v>5.62</v>
+      </c>
+      <c r="P8" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="R8" t="n">
+        <v>7.03</v>
+      </c>
+      <c r="S8" t="n">
+        <v>5.9058332</v>
+      </c>
+      <c r="T8" t="n">
+        <v>5.7478013</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>SKY</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>65</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-4939.349999999999</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4939.349999999999</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Skyline Champion Corporation</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>1105.65007686615</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2018-05-24</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>75.33</v>
+      </c>
+      <c r="N9" t="n">
+        <v>75.98999999999999</v>
+      </c>
+      <c r="O9" t="n">
+        <v>74.56</v>
+      </c>
+      <c r="P9" t="n">
+        <v>76.34</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>28.73</v>
+      </c>
+      <c r="R9" t="n">
+        <v>77.40000000000001</v>
+      </c>
+      <c r="S9" t="n">
+        <v>64.97360999999999</v>
+      </c>
+      <c r="T9" t="n">
+        <v>56.778652</v>
+      </c>
+      <c r="U9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NYMX</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>3012</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-4999.92</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4999.92</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nymox Pharmaceutical Corporation</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>2680.680315971375</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
         <v>1.76</v>
       </c>
-      <c r="N2" t="n">
-        <v>1.812</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1.76</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1.88</v>
-      </c>
-      <c r="Q2" t="n">
+      <c r="N10" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="Q10" t="n">
         <v>1.25</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R10" t="n">
         <v>3.5</v>
       </c>
-      <c r="S2" t="n">
-        <v>1.955</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1.7909353</v>
-      </c>
-      <c r="U2" t="inlineStr"/>
+      <c r="S10" t="n">
+        <v>1.9277778</v>
+      </c>
+      <c r="T10" t="n">
+        <v>1.7875886</v>
+      </c>
+      <c r="U10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added a disorganized way of using trained model on untrained year and fixed the transaction builder
</commit_message>
<xml_diff>
--- a/datatickers123.xlsx
+++ b/datatickers123.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +531,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -541,14 +541,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>XBIT</t>
+          <t>KB</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1142</v>
+        <v>120</v>
       </c>
       <c r="F2" t="n">
-        <v>4.377177715301514</v>
+        <v>41.36999893188477</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -560,19 +560,19 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>-4998.736950874329</v>
+        <v>-4964.399871826172</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1250</v>
+        <v>121.9512195121951</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>4998.736950874329</v>
+        <v>4964.399871826172</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -587,54 +587,314 @@
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>4.377177715301514</v>
+        <v>41.36999893188477</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CIB</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>94</v>
+      </c>
+      <c r="F3" t="n">
+        <v>52.711181640625</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-4954.85107421875</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>96.15384615384616</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>4954.85107421875</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>52.711181640625</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>AVAL</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>619</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8.075420379638672</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-4998.685214996338</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>625</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>4998.685214996338</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>8.075420379638672</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>DMTK</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>403</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12.39999961853027</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-4997.1998462677</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>416.6666666666667</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>4997.1998462677</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>12.39999961853027</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>GLBD</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>2941</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.700000047683716</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-4999.700140237808</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>5000</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>4999.700140237808</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1.700000047683716</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>